<commit_message>
Projet d'algebres initialisation du depot
</commit_message>
<xml_diff>
--- a/Exercice_4/Question 2.xlsx
+++ b/Exercice_4/Question 2.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Oumar\Ordinateur Dell\oumar\documents\Cours\IA data forest\master semestre 1\Calcul matriciel\Projet Algèbres\Exercice_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD50118-050C-4825-A194-6B9729D4BA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1F6901-092F-4F89-BB46-A4C685A23DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Feuil1!$D$3,Feuil1!$D$4</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Feuil1!$E$3,Feuil1!$E$4</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
@@ -32,7 +32,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Feuil1!$D$6</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Feuil1!$E$6</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Valeurs </t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>x2 &gt;= 0</t>
+  </si>
+  <si>
+    <t>Résultats</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <dimension ref="C1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,18 +538,25 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
         <v>1.4545454545454546</v>
       </c>
     </row>
@@ -555,6 +565,9 @@
         <v>3</v>
       </c>
       <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
         <v>1.9090909090909092</v>
       </c>
     </row>
@@ -563,6 +576,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
@@ -570,6 +584,10 @@
       </c>
       <c r="D6" s="5">
         <f>4*D3+3*D4</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <f>4*E3+3*E4</f>
         <v>11.545454545454547</v>
       </c>
     </row>
@@ -592,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="9">
-        <f>3*D3+4*D4</f>
+        <f>3*E3+4*E4</f>
         <v>12</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -607,7 +625,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="9">
-        <f>7*D3+2*D4</f>
+        <f>7*E3+2*E4</f>
         <v>14</v>
       </c>
       <c r="E10" s="7" t="s">

</xml_diff>